<commit_message>
Corrected font_properties excel files.
</commit_message>
<xml_diff>
--- a/mcw_readers/data/all_versions_meta_information.xlsx
+++ b/mcw_readers/data/all_versions_meta_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\mcwcorp\Departments\Neurology\Users\jheffernan\ForOthers\lumfleet\neuroscore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4670CE-4683-4D6B-8B31-22127B9B1DCC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3625B4CE-BE60-4D47-895A-F8B28CAA87F8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25680" yWindow="1788" windowWidth="23040" windowHeight="12660" xr2:uid="{D7196569-49B9-4FDA-ABC4-A46F44C16361}"/>
+    <workbookView xWindow="1632" yWindow="2904" windowWidth="23040" windowHeight="12660" xr2:uid="{D7196569-49B9-4FDA-ABC4-A46F44C16361}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -447,7 +447,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -612,7 +612,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
@@ -626,7 +626,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -640,7 +640,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -654,13 +654,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
@@ -668,13 +668,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
       <c r="C16">
-        <v>708</v>
+        <v>739</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
@@ -682,7 +682,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
@@ -696,7 +696,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -710,7 +710,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
@@ -724,7 +724,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
@@ -738,13 +738,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
         <v>15</v>
       </c>
       <c r="C21">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D21" t="s">
         <v>12</v>
@@ -752,7 +752,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
@@ -766,7 +766,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -780,7 +780,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
@@ -794,7 +794,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
         <v>11</v>
@@ -808,13 +808,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
         <v>15</v>
       </c>
       <c r="C26">
-        <v>726</v>
+        <v>709</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
@@ -822,7 +822,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
@@ -836,7 +836,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -850,7 +850,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
         <v>9</v>
@@ -864,7 +864,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
@@ -878,7 +878,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B31" t="s">
         <v>15</v>
@@ -892,7 +892,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B32" t="s">
         <v>5</v>
@@ -906,7 +906,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
         <v>7</v>
@@ -920,7 +920,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B34" t="s">
         <v>9</v>
@@ -934,13 +934,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
         <v>11</v>
       </c>
       <c r="C35">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D35" t="s">
         <v>12</v>
@@ -948,13 +948,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B36" t="s">
         <v>15</v>
       </c>
       <c r="C36">
-        <v>739</v>
+        <v>726</v>
       </c>
       <c r="D36" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Corrcted the meta data excel file for all neuroscore versions.
</commit_message>
<xml_diff>
--- a/mcw_readers/data/all_versions_meta_information.xlsx
+++ b/mcw_readers/data/all_versions_meta_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\mcwcorp\Departments\Neurology\Users\jheffernan\ForOthers\lumfleet\neuroscore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3625B4CE-BE60-4D47-895A-F8B28CAA87F8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30DFAEB-36DF-4471-810D-750FA7BE9249}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1632" yWindow="2904" windowWidth="23040" windowHeight="12660" xr2:uid="{D7196569-49B9-4FDA-ABC4-A46F44C16361}"/>
+    <workbookView xWindow="1608" yWindow="2628" windowWidth="23040" windowHeight="12660" xr2:uid="{D7196569-49B9-4FDA-ABC4-A46F44C16361}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -447,7 +447,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -744,7 +744,7 @@
         <v>15</v>
       </c>
       <c r="C21">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="D21" t="s">
         <v>12</v>

</xml_diff>